<commit_message>
add “buy currency” example
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/currencyExchange.xlsx
+++ b/src/main/webapp/WEB-INF/book/currencyExchange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD2C322-4CA4-F64A-B267-66A71A94BA8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF7F1FF-F329-6240-9990-3417EC04EEFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35860" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{0F9DCD2C-5658-5540-A68B-4E38358CBFB3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="select" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,10 @@
     <sheet name="list" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">list!$A$2:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">list!#REF!</definedName>
+    <definedName name="amount">exchange!$G$7</definedName>
+    <definedName name="cost">exchange!$D$7</definedName>
+    <definedName name="rate">exchange!$G$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,40 +33,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>=</t>
-  </si>
-  <si>
-    <t>Select your destination country/currency:</t>
-  </si>
-  <si>
-    <t>Buy Currency online</t>
-  </si>
-  <si>
-    <t>how much would you buy</t>
   </si>
   <si>
     <t>Rate</t>
   </si>
   <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>How much would you buy?</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Local Amount</t>
+  </si>
+  <si>
+    <t>Foreign Amount</t>
+  </si>
+  <si>
     <t>Currency</t>
   </si>
   <si>
-    <t>EUR</t>
+    <t>New Zealand</t>
   </si>
   <si>
-    <t>Currency Amount</t>
+    <t>Canada</t>
   </si>
   <si>
-    <t>Cost</t>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Buy Currency Online</t>
+  </si>
+  <si>
+    <t>Click to select your destination country/currency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,12 +117,126 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF3598DB"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial Bold"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00C3F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00C3F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF33495E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Arial Bold"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Bold"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,12 +245,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FFF4F4F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33495E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00C3F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,29 +282,412 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00C3F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF00C3F0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" textRotation="0" wrapText="0" relativeIndent="-1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Arial Bold"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF00C3F0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="-1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="2" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="2" tint="-0.24994659260841701"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="2" tint="-0.24994659260841701"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="medium">
+          <color theme="2" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="medium">
+          <color theme="2" tint="-0.499984740745262"/>
+        </bottom>
+        <horizontal style="medium">
+          <color theme="2" tint="-0.499984740745262"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFF4F4F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="9" tint="0.79995117038483843"/>
+          <bgColor rgb="FFF4F4F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="totalRow" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
+    </tableStyle>
+    <tableStyle name="Table Style 2" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}"/>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF00C3F0"/>
+      <color rgb="FF33495E"/>
+      <color rgb="FFF4F4F4"/>
+      <color rgb="FF3598DB"/>
+      <color rgb="FFEEEEEE"/>
+      <color rgb="FF2FB5B6"/>
+      <color rgb="FFD6E7F0"/>
+      <color rgb="FFE3F0FE"/>
+      <color rgb="FF393E46"/>
+      <color rgb="FFF1C313"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -152,30 +709,85 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="101600" y="1536700"/>
+          <a:ext cx="1092200" cy="1092200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>101600</xdr:colOff>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>800100</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>660400</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>139700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Buy" hidden="1">
+            <xdr:cNvPr id="2050" name="Buy" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
+                  <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -208,8 +820,9 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                  <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                  <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Buy</a:t>
               </a:r>
@@ -224,22 +837,22 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>1422400</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>50800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>685800</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>508000</xdr:rowOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>444500</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -282,8 +895,9 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
-                  <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                  <a:latin typeface="Verdana" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="Verdana" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Verdana" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Buy Another</a:t>
               </a:r>
@@ -296,6 +910,31 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="F8:H15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Country" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Currency" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Rate" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="C5:G6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="C5:G6" xr:uid="{0A78C6CE-FDBA-0547-9169-45A405A5CFB1}"/>
+  <tableColumns count="5">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Date" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Local Amount" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Currency" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Rate" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Foreign Amount" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,101 +1233,929 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B792991-CE23-4249-8770-2DCB62345E69}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="5" width="2.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" customWidth="1"/>
+    <col min="12" max="12" width="1.83203125" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="2" spans="2:15" ht="83" customHeight="1">
+      <c r="B2" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+    </row>
+    <row r="3" spans="2:15" ht="6" customHeight="1">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="2:15" ht="36" customHeight="1">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="B5" s="11"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="10"/>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" s="11"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="10"/>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" spans="2:15" ht="23" customHeight="1">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="34" t="s">
         <v>1</v>
       </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="10"/>
+    </row>
+    <row r="9" spans="2:15" ht="23" customHeight="1">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="10"/>
+    </row>
+    <row r="10" spans="2:15" ht="23" customHeight="1">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" spans="2:15" ht="23" customHeight="1">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" spans="2:15" ht="23" customHeight="1">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" spans="2:15" ht="23" customHeight="1">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" spans="2:15" ht="23" customHeight="1">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+    </row>
+    <row r="15" spans="2:15" ht="23" customHeight="1">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" spans="2:15" ht="55" customHeight="1">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+    </row>
+    <row r="17" spans="2:14" ht="23" customHeight="1">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="2:14" ht="23" customHeight="1">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="2:14" ht="23" customHeight="1">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="2:14" ht="23" customHeight="1">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="2:14" ht="23" customHeight="1">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="2:14" ht="23" customHeight="1">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="2:14" ht="23" customHeight="1">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="2:14" ht="23" customHeight="1">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="2:14" ht="23" customHeight="1">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="2:14" ht="23" customHeight="1">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="2:14" ht="23" customHeight="1">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="2:14" ht="23" customHeight="1">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="2:14" ht="23" customHeight="1">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="2:14" ht="23" customHeight="1">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="2:14" ht="23" customHeight="1">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+    </row>
+    <row r="32" spans="2:14" ht="23" customHeight="1">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+    </row>
+    <row r="33" spans="2:14" ht="23" customHeight="1">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+    </row>
+    <row r="34" spans="2:14" ht="23" customHeight="1">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+    </row>
+    <row r="35" spans="2:14" ht="23" customHeight="1">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+    </row>
+    <row r="36" spans="2:14" ht="23" customHeight="1">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+    </row>
+    <row r="37" spans="2:14" ht="23" customHeight="1">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+    </row>
+    <row r="38" spans="2:14" ht="23" customHeight="1">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+    </row>
+    <row r="39" spans="2:14" ht="23" customHeight="1">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I5:K6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F818F4D-BF3C-544A-B28E-D5CCC1235EF9}">
-  <dimension ref="B2:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="6" width="5.5" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:16" ht="83" customHeight="1">
+      <c r="B2" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+    </row>
+    <row r="3" spans="1:16" ht="6" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1">
+      <c r="B4" s="21"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="B5" s="10"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="68" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="7"/>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" ht="17" customHeight="1">
+      <c r="B6" s="10"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:16" ht="20" customHeight="1" thickBot="1">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
-        <f>B3*E4</f>
+      <c r="G7" s="59">
+        <f>D7*G9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4">
+      <c r="H7" s="60" t="str">
+        <f>H9</f>
+        <v>USD</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" ht="10" customHeight="1">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="57">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E9" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="G9" s="58">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H9" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" ht="13" customHeight="1">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" ht="17" customHeight="1">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="B16" s="4"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="3"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="D5:G6"/>
+    <mergeCell ref="C16:F17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId3" name="Buy">
+            <control shapeId="2050" r:id="rId4" name="Buy">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>101600</xdr:colOff>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>800100</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>660400</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>139700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -702,39 +2169,238 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB057893-6B77-9E4B-A23F-9146BB2E0E62}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
-    <col min="3" max="3" width="10.83203125" style="3"/>
-    <col min="4" max="4" width="18.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" customWidth="1"/>
+    <col min="10" max="10" width="3" customWidth="1"/>
+    <col min="11" max="11" width="4.5" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:13" ht="83" customHeight="1">
+      <c r="B2" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+    </row>
+    <row r="3" spans="1:13" ht="6" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:13" ht="36" customHeight="1">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" ht="23" customHeight="1">
+      <c r="B5" s="23"/>
+      <c r="C5" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:13" ht="23" customHeight="1">
+      <c r="B6" s="23"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:13" ht="61" customHeight="1">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" ht="29" customHeight="1">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" autoFilter="0"/>
-  <autoFilter ref="A2:D2" xr:uid="{ABB3F362-588B-EB4D-B3D1-0766441356A4}"/>
+  <sheetProtection sheet="1" autoFilter="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B2:L2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -747,16 +2413,16 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>1422400</xdr:colOff>
-                    <xdr:row>0</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>50800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>685800</xdr:colOff>
-                    <xdr:row>0</xdr:row>
-                    <xdr:rowOff>508000</xdr:rowOff>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>444500</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -766,5 +2432,8 @@
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
protect sheets with UserInterfaceOnly instead of unprotect + protect
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/currencyExchange.xlsx
+++ b/src/main/webapp/WEB-INF/book/currencyExchange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF7F1FF-F329-6240-9990-3417EC04EEFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A575B83-B8FC-A541-A52F-005CE2021B34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="select" sheetId="1" r:id="rId1"/>
@@ -1883,7 +1883,6 @@
       <c r="N41" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B2:N2"/>
@@ -1903,7 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:P18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2172,7 +2171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:M15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2397,7 +2396,7 @@
       <c r="M15" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" autoFilter="0"/>
+  <sheetProtection autoFilter="0"/>
   <mergeCells count="1">
     <mergeCell ref="B2:L2"/>
   </mergeCells>

</xml_diff>